<commit_message>
depployment first try finished
</commit_message>
<xml_diff>
--- a/static/document/experience.xlsx
+++ b/static/document/experience.xlsx
@@ -144,14 +144,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Make manual test product line become a automatic test product line.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>This website.CV display.Skills document collection.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Back-end data process.React front-end build.Dynamic validation features.Dynamic trend charts</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -196,7 +188,15 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Quick screen shot.Quick translation.Quick take text from picture.Quick Highlight.Quick picture formate transform.</t>
+    <t>This website.CV display.Skills document collection</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Quick screen shot.Quick translation.Quick take text from picture.Quick Highlight.Quick picture formate transform</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Make manual test product line become a automatic test product line</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -565,7 +565,7 @@
   <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+      <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -599,7 +599,7 @@
         <v>5</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="2" spans="1:7">
@@ -616,7 +616,7 @@
         <v>8</v>
       </c>
       <c r="E2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="F2" t="s">
         <v>23</v>
@@ -662,7 +662,7 @@
         <v>7</v>
       </c>
       <c r="E4" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="F4" t="s">
         <v>25</v>
@@ -708,13 +708,13 @@
         <v>7</v>
       </c>
       <c r="E6" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="F6" t="s">
         <v>27</v>
       </c>
       <c r="G6" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="7" spans="1:7">
@@ -731,13 +731,13 @@
         <v>7</v>
       </c>
       <c r="E7" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="F7" t="s">
+        <v>44</v>
+      </c>
+      <c r="G7" t="s">
         <v>46</v>
-      </c>
-      <c r="G7" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="8" spans="1:7">
@@ -754,13 +754,13 @@
         <v>16</v>
       </c>
       <c r="E8" t="s">
+        <v>43</v>
+      </c>
+      <c r="F8" t="s">
         <v>45</v>
       </c>
-      <c r="F8" t="s">
+      <c r="G8" t="s">
         <v>47</v>
-      </c>
-      <c r="G8" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="9" spans="1:7">
@@ -783,7 +783,7 @@
         <v>28</v>
       </c>
       <c r="G9" t="s">
-        <v>35</v>
+        <v>48</v>
       </c>
     </row>
     <row r="10" spans="1:7">
@@ -800,13 +800,13 @@
         <v>16</v>
       </c>
       <c r="E10" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="F10" t="s">
         <v>32</v>
       </c>
       <c r="G10" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
   </sheetData>

</xml_diff>